<commit_message>
workflow chart and README.md
</commit_message>
<xml_diff>
--- a/database/banking_data.xlsx
+++ b/database/banking_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lituokobe/Desktop/Digital_Banking_Chatbot/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FC9AB0-08CB-214C-8566-F5AF54C906C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A68A00D-01D9-4640-947C-692EA9F2370E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16000" yWindow="2500" windowWidth="22400" windowHeight="18720" firstSheet="3" activeTab="10" xr2:uid="{9300CA19-CC8C-5C49-AD0F-B8AC562857F7}"/>
+    <workbookView xWindow="15760" yWindow="2880" windowWidth="22400" windowHeight="18720" xr2:uid="{9300CA19-CC8C-5C49-AD0F-B8AC562857F7}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="127">
   <si>
     <t>user_id</t>
   </si>
@@ -91,15 +91,9 @@
     <t>HN68</t>
   </si>
   <si>
-    <t>Amariano</t>
-  </si>
-  <si>
     <t>Jun-Hao</t>
   </si>
   <si>
-    <t>Mutobikkavos</t>
-  </si>
-  <si>
     <t>Satsuki</t>
   </si>
   <si>
@@ -416,6 +410,24 @@
   </si>
   <si>
     <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>Mariano</t>
+  </si>
+  <si>
+    <t>Ukeja</t>
   </si>
 </sst>
 </file>
@@ -799,23 +811,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D05990-E6A8-2547-9872-0C7BC54C09A6}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -826,22 +840,28 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -851,95 +871,119 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
+        <v>34832</v>
+      </c>
+      <c r="E2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2">
         <v>2009</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>1996</v>
+      <c r="D3" s="1">
+        <v>38258</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3">
+        <v>2022</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>2021</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>23730</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4">
+        <v>1996</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1">
+        <v>30470</v>
+      </c>
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5">
         <v>2017</v>
       </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
-        <v>41</v>
+      <c r="I5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -963,13 +1007,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1014,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9D7DF3-F7AE-C843-9BB8-17789036BA45}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1028,31 +1072,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>87</v>
-      </c>
-      <c r="F1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1060,13 +1104,13 @@
         <v>45918</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E2">
         <v>72</v>
@@ -1092,13 +1136,13 @@
         <v>45918</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E3">
         <v>155</v>
@@ -1124,13 +1168,13 @@
         <v>45918</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4">
         <v>180</v>
@@ -1156,13 +1200,13 @@
         <v>45918</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E5">
         <v>80</v>
@@ -1188,13 +1232,13 @@
         <v>45918</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E6">
         <v>86</v>
@@ -1239,22 +1283,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
         <v>105</v>
-      </c>
-      <c r="F1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1262,16 +1306,16 @@
         <v>45919</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2">
         <v>500</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F2" s="1">
         <v>45919</v>
@@ -1282,16 +1326,16 @@
         <v>45919</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>1500</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F3" s="1">
         <v>45919</v>
@@ -1302,16 +1346,16 @@
         <v>45919</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>300</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F4" s="5">
         <v>45932</v>
@@ -1322,16 +1366,16 @@
         <v>45919</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>6000</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F5" s="5">
         <v>45929</v>
@@ -1363,16 +1407,16 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1380,16 +1424,16 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>2025</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1397,16 +1441,16 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>2002</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1414,16 +1458,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>2014</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1450,19 +1494,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1470,7 +1514,7 @@
         <v>45792</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>2200</v>
@@ -1479,7 +1523,7 @@
         <v>2200</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1487,7 +1531,7 @@
         <v>45797</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>-58.6</v>
@@ -1497,7 +1541,7 @@
         <v>2141.4</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1505,7 +1549,7 @@
         <v>45800</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>-1200</v>
@@ -1515,7 +1559,7 @@
         <v>941.40000000000009</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1523,7 +1567,7 @@
         <v>45802</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>3.4</v>
@@ -1533,7 +1577,7 @@
         <v>944.80000000000007</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1541,7 +1585,7 @@
         <v>45814</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>-180</v>
@@ -1551,7 +1595,7 @@
         <v>764.80000000000007</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1559,7 +1603,7 @@
         <v>45823</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2">
         <v>1600</v>
@@ -1569,7 +1613,7 @@
         <v>2364.8000000000002</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1577,7 +1621,7 @@
         <v>45825</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>-85.4</v>
@@ -1587,7 +1631,7 @@
         <v>2279.4</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1595,7 +1639,7 @@
         <v>45826</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9">
         <v>-66</v>
@@ -1605,7 +1649,7 @@
         <v>2213.4</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1613,7 +1657,7 @@
         <v>45828</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>-300</v>
@@ -1623,7 +1667,7 @@
         <v>1913.4</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1631,7 +1675,7 @@
         <v>45833</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>4.75</v>
@@ -1641,7 +1685,7 @@
         <v>1918.15</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1649,7 +1693,7 @@
         <v>45836</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>-92.1</v>
@@ -1659,7 +1703,7 @@
         <v>1826.0500000000002</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1667,7 +1711,7 @@
         <v>45839</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>450</v>
@@ -1677,7 +1721,7 @@
         <v>2276.0500000000002</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1685,7 +1729,7 @@
         <v>45841</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>-120</v>
@@ -1695,7 +1739,7 @@
         <v>2156.0500000000002</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1703,7 +1747,7 @@
         <v>45843</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15">
         <v>-500</v>
@@ -1713,7 +1757,7 @@
         <v>1656.0500000000002</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1721,7 +1765,7 @@
         <v>45848</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>-60</v>
@@ -1731,7 +1775,7 @@
         <v>1596.0500000000002</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1739,7 +1783,7 @@
         <v>45850</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C17">
         <v>-312</v>
@@ -1749,7 +1793,7 @@
         <v>1284.0500000000002</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1757,7 +1801,7 @@
         <v>45853</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2">
         <v>2400</v>
@@ -1767,7 +1811,7 @@
         <v>3684.05</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1775,7 +1819,7 @@
         <v>45856</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19">
         <v>-75.3</v>
@@ -1785,7 +1829,7 @@
         <v>3608.75</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1793,7 +1837,7 @@
         <v>45863</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20">
         <v>5.0999999999999996</v>
@@ -1803,7 +1847,7 @@
         <v>3613.85</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1811,7 +1855,7 @@
         <v>45868</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C21">
         <v>-250</v>
@@ -1821,7 +1865,7 @@
         <v>3363.85</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1829,7 +1873,7 @@
         <v>45870</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C22">
         <v>80</v>
@@ -1839,7 +1883,7 @@
         <v>3443.85</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1847,7 +1891,7 @@
         <v>45874</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23">
         <v>-45</v>
@@ -1857,7 +1901,7 @@
         <v>3398.85</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1865,7 +1909,7 @@
         <v>45879</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24">
         <v>-200</v>
@@ -1875,7 +1919,7 @@
         <v>3198.85</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1883,7 +1927,7 @@
         <v>45884</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25" s="2">
         <v>1800</v>
@@ -1893,7 +1937,7 @@
         <v>4998.8500000000004</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1901,7 +1945,7 @@
         <v>45889</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26">
         <v>-196</v>
@@ -1911,7 +1955,7 @@
         <v>4802.8500000000004</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1919,7 +1963,7 @@
         <v>45894</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27">
         <v>5.3</v>
@@ -1929,7 +1973,7 @@
         <v>4808.1500000000005</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1937,7 +1981,7 @@
         <v>45910</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <v>-850</v>
@@ -1947,7 +1991,7 @@
         <v>3958.1500000000005</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1974,19 +2018,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1994,7 +2038,7 @@
         <v>45809</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2">
         <v>1500</v>
@@ -2003,7 +2047,7 @@
         <v>1500</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2011,7 +2055,7 @@
         <v>45811</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>-9.25</v>
@@ -2020,7 +2064,7 @@
         <v>1490.75</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2028,7 +2072,7 @@
         <v>45813</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4">
         <v>-150</v>
@@ -2037,7 +2081,7 @@
         <v>1340.75</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2045,7 +2089,7 @@
         <v>45815</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>-900</v>
@@ -2054,7 +2098,7 @@
         <v>440.75</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2062,7 +2106,7 @@
         <v>45818</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>1.8</v>
@@ -2071,7 +2115,7 @@
         <v>442.55</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2079,7 +2123,7 @@
         <v>45820</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7">
         <v>-7.5</v>
@@ -2088,7 +2132,7 @@
         <v>435.05</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2096,7 +2140,7 @@
         <v>45823</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>500</v>
@@ -2105,7 +2149,7 @@
         <v>935.05</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2113,7 +2157,7 @@
         <v>45826</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>-40</v>
@@ -2122,7 +2166,7 @@
         <v>895.05</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2130,7 +2174,7 @@
         <v>45828</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10">
         <v>-18</v>
@@ -2139,7 +2183,7 @@
         <v>877.05</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2147,7 +2191,7 @@
         <v>45833</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>1.9</v>
@@ -2156,7 +2200,7 @@
         <v>878.95</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2164,7 +2208,7 @@
         <v>45836</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12">
         <v>-60</v>
@@ -2173,7 +2217,7 @@
         <v>818.95</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2181,7 +2225,7 @@
         <v>45839</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="2">
         <v>1500</v>
@@ -2190,7 +2234,7 @@
         <v>2318.9499999999998</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2198,7 +2242,7 @@
         <v>45841</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14">
         <v>-80</v>
@@ -2207,7 +2251,7 @@
         <v>2238.9499999999998</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2215,7 +2259,7 @@
         <v>45843</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15">
         <v>-900</v>
@@ -2224,7 +2268,7 @@
         <v>1338.95</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2232,7 +2276,7 @@
         <v>45848</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -2241,7 +2285,7 @@
         <v>1340.95</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2249,7 +2293,7 @@
         <v>45853</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C17">
         <v>500</v>
@@ -2258,7 +2302,7 @@
         <v>1840.95</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2266,7 +2310,7 @@
         <v>45856</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18">
         <v>-30</v>
@@ -2275,7 +2319,7 @@
         <v>1810.95</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2283,7 +2327,7 @@
         <v>45858</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19">
         <v>-15</v>
@@ -2292,7 +2336,7 @@
         <v>1795.95</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2300,7 +2344,7 @@
         <v>45863</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20">
         <v>2.1</v>
@@ -2309,7 +2353,7 @@
         <v>1798.05</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2317,7 +2361,7 @@
         <v>45868</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21">
         <v>-600</v>
@@ -2326,7 +2370,7 @@
         <v>1198.05</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2353,19 +2397,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2373,7 +2417,7 @@
         <v>45809</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2">
         <v>2800</v>
@@ -2382,7 +2426,7 @@
         <v>2800</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2390,7 +2434,7 @@
         <v>45811</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>-45</v>
@@ -2399,7 +2443,7 @@
         <v>2755</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2407,7 +2451,7 @@
         <v>45813</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>-110.25</v>
@@ -2416,7 +2460,7 @@
         <v>2644.75</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2424,7 +2468,7 @@
         <v>45815</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>-500</v>
@@ -2433,7 +2477,7 @@
         <v>2144.75</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2441,7 +2485,7 @@
         <v>45818</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>3.1</v>
@@ -2450,7 +2494,7 @@
         <v>2147.85</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2458,7 +2502,7 @@
         <v>45823</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>-60</v>
@@ -2467,7 +2511,7 @@
         <v>2087.85</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2475,7 +2519,7 @@
         <v>45828</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>-95</v>
@@ -2484,7 +2528,7 @@
         <v>1992.85</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2492,7 +2536,7 @@
         <v>45833</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2">
         <v>2800</v>
@@ -2501,7 +2545,7 @@
         <v>4792.8500000000004</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2509,7 +2553,7 @@
         <v>45836</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10">
         <v>-100</v>
@@ -2518,7 +2562,7 @@
         <v>4692.8500000000004</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2526,7 +2570,7 @@
         <v>45839</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11">
         <v>-40</v>
@@ -2535,7 +2579,7 @@
         <v>4652.8500000000004</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2543,7 +2587,7 @@
         <v>45843</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>-700</v>
@@ -2552,7 +2596,7 @@
         <v>3952.85</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2560,7 +2604,7 @@
         <v>45848</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13">
         <v>3.25</v>
@@ -2569,7 +2613,7 @@
         <v>3956.1</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2577,7 +2621,7 @@
         <v>45853</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2">
         <v>2800</v>
@@ -2586,7 +2630,7 @@
         <v>6756.1</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2594,7 +2638,7 @@
         <v>45856</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15">
         <v>-115</v>
@@ -2603,7 +2647,7 @@
         <v>6641.1</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2611,7 +2655,7 @@
         <v>45858</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16">
         <v>-200</v>
@@ -2620,7 +2664,7 @@
         <v>6441.1</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2628,7 +2672,7 @@
         <v>45863</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2">
         <v>-1000</v>
@@ -2637,7 +2681,7 @@
         <v>5441.1</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2645,7 +2689,7 @@
         <v>45866</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18">
         <v>-70</v>
@@ -2654,7 +2698,7 @@
         <v>5371.1</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2662,7 +2706,7 @@
         <v>45870</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" s="2">
         <v>2800</v>
@@ -2671,7 +2715,7 @@
         <v>8171.1</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2679,7 +2723,7 @@
         <v>45874</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C20">
         <v>-350</v>
@@ -2688,7 +2732,7 @@
         <v>7821.1</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2696,7 +2740,7 @@
         <v>45879</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21">
         <v>3.4</v>
@@ -2705,7 +2749,7 @@
         <v>7824.5</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2732,19 +2776,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2752,7 +2796,7 @@
         <v>45809</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>4500</v>
@@ -2761,7 +2805,7 @@
         <v>4500</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2769,7 +2813,7 @@
         <v>45811</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>-6.75</v>
@@ -2778,7 +2822,7 @@
         <v>4493.25</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2786,7 +2830,7 @@
         <v>45813</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>-120.4</v>
@@ -2795,7 +2839,7 @@
         <v>4372.8500000000004</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2803,7 +2847,7 @@
         <v>45815</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2">
         <v>-1000</v>
@@ -2812,7 +2856,7 @@
         <v>3372.85</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2820,7 +2864,7 @@
         <v>45818</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>4.25</v>
@@ -2829,7 +2873,7 @@
         <v>3377.1</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2837,7 +2881,7 @@
         <v>45820</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>-65</v>
@@ -2846,7 +2890,7 @@
         <v>3312.1</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2854,7 +2898,7 @@
         <v>45823</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>600</v>
@@ -2863,7 +2907,7 @@
         <v>3912.1</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2871,7 +2915,7 @@
         <v>45826</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9">
         <v>-75.2</v>
@@ -2880,7 +2924,7 @@
         <v>3836.9</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2888,7 +2932,7 @@
         <v>45828</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>-300</v>
@@ -2897,7 +2941,7 @@
         <v>3536.9</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2905,7 +2949,7 @@
         <v>45833</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>4.5</v>
@@ -2914,7 +2958,7 @@
         <v>3541.4</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2922,7 +2966,7 @@
         <v>45839</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2">
         <v>4500</v>
@@ -2931,7 +2975,7 @@
         <v>8041.4</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2939,7 +2983,7 @@
         <v>45841</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13">
         <v>-150</v>
@@ -2948,7 +2992,7 @@
         <v>7891.4</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2956,7 +3000,7 @@
         <v>45843</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>-60</v>
@@ -2965,7 +3009,7 @@
         <v>7831.4</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2973,7 +3017,7 @@
         <v>45848</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2">
         <v>-1200</v>
@@ -2982,7 +3026,7 @@
         <v>6631.4</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2990,7 +3034,7 @@
         <v>45853</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <v>-80</v>
@@ -2999,7 +3043,7 @@
         <v>6551.4</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3007,7 +3051,7 @@
         <v>45858</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17">
         <v>-450</v>
@@ -3016,7 +3060,7 @@
         <v>6101.4</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3024,7 +3068,7 @@
         <v>45863</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18">
         <v>4.75</v>
@@ -3033,7 +3077,7 @@
         <v>6106.15</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -3041,7 +3085,7 @@
         <v>45870</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2">
         <v>4500</v>
@@ -3050,7 +3094,7 @@
         <v>10606.15</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3058,7 +3102,7 @@
         <v>45874</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20">
         <v>-800</v>
@@ -3067,7 +3111,7 @@
         <v>9806.15</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -3075,7 +3119,7 @@
         <v>45879</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>-130.6</v>
@@ -3084,7 +3128,7 @@
         <v>9675.5499999999993</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -3110,34 +3154,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
         <v>86</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" t="s">
-        <v>89</v>
-      </c>
       <c r="I1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3145,10 +3189,10 @@
         <v>45789</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2">
         <v>395.94</v>
@@ -3181,10 +3225,10 @@
         <v>45799</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3">
         <v>414.33</v>
@@ -3218,10 +3262,10 @@
         <v>45810</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4">
         <v>201.7</v>
@@ -3255,10 +3299,10 @@
         <v>45811</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>141.22</v>
@@ -3292,10 +3336,10 @@
         <v>45819</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6">
         <v>412.84</v>
@@ -3329,10 +3373,10 @@
         <v>45820</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7">
         <v>145</v>
@@ -3366,10 +3410,10 @@
         <v>45826</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8">
         <v>145.47999999999999</v>
@@ -3403,10 +3447,10 @@
         <v>45859</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D9">
         <v>171.38</v>
@@ -3440,10 +3484,10 @@
         <v>45863</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D10">
         <v>213.88</v>
@@ -3477,10 +3521,10 @@
         <v>45870</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D11">
         <v>173.72</v>
@@ -3556,34 +3600,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
         <v>86</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" t="s">
-        <v>89</v>
-      </c>
       <c r="I1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3591,10 +3635,10 @@
         <v>45838</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2">
         <v>91.63</v>
@@ -3627,10 +3671,10 @@
         <v>45839</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3">
         <v>94.92</v>
@@ -3664,10 +3708,10 @@
         <v>45841</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4">
         <v>76.39</v>
@@ -3701,10 +3745,10 @@
         <v>45846</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>73.92</v>
@@ -3738,10 +3782,10 @@
         <v>45880</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6">
         <v>91.74</v>
@@ -3775,10 +3819,10 @@
         <v>45895</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7">
         <v>78.650000000000006</v>
@@ -3812,10 +3856,10 @@
         <v>45916</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8">
         <v>84.37</v>
@@ -3865,34 +3909,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
         <v>86</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" t="s">
-        <v>89</v>
-      </c>
       <c r="I1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3900,10 +3944,10 @@
         <v>45818</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2">
         <v>534.21</v>
@@ -3936,10 +3980,10 @@
         <v>45824</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3">
         <v>534.29</v>
@@ -3973,10 +4017,10 @@
         <v>45840</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4">
         <v>550.79999999999995</v>
@@ -4010,10 +4054,10 @@
         <v>45852</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5">
         <v>556.21</v>
@@ -4047,10 +4091,10 @@
         <v>45875</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6">
         <v>576.32000000000005</v>
@@ -4084,10 +4128,10 @@
         <v>45894</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7">
         <v>570.32000000000005</v>
@@ -4121,10 +4165,10 @@
         <v>45910</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8">
         <v>580.70000000000005</v>

</xml_diff>